<commit_message>
feat: add output section in module.exports for webpack configs
</commit_message>
<xml_diff>
--- a/4 - Build Tools and Single Page Web Apps/Project_04_Rubric.xlsx
+++ b/4 - Build Tools and Single Page Web Apps/Project_04_Rubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danihergar/Documents/Repositories/udacity_Front_End_Web_Developer/4 - Build Tools and Single Page Web Apps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4612CE55-2F60-A844-8ACB-09D711174B68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69206A1C-EBAA-3049-8DBD-6503F35D3B03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="460" windowWidth="27760" windowHeight="16000" xr2:uid="{DB850500-CB71-2948-A340-54DF47885E39}"/>
   </bookViews>
@@ -126,7 +126,7 @@
       <name val="Open Sans"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,6 +142,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -173,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -181,13 +187,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -507,7 +519,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -517,10 +529,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="20">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="5"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
@@ -531,34 +543,34 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="171">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="95">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="114">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="20">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="5"/>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
@@ -569,34 +581,34 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="95">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="19">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="19">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="76">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>